<commit_message>
updated default tiers and added missing types
</commit_message>
<xml_diff>
--- a/app/shiny/templates/order_tier_defaults.xlsx
+++ b/app/shiny/templates/order_tier_defaults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\DesktopDeployR\app\shiny\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5991F4B1-7DB6-401F-B072-21F388DA7B36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597F9639-B8E3-4160-9A5B-E8708AE5FFAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="1995" windowWidth="21015" windowHeight="13755" xr2:uid="{BC889A8F-D699-4C57-8F41-18B70471A466}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="22680" windowHeight="12240" xr2:uid="{BC889A8F-D699-4C57-8F41-18B70471A466}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>type</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>behavioral health clinic</t>
+  </si>
+  <si>
+    <t>Chiropractic</t>
+  </si>
+  <si>
+    <t>Dialysis</t>
   </si>
 </sst>
 </file>
@@ -480,11 +486,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B3EFE4-6916-41B6-9807-EC4A4D8D59DA}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -662,7 +666,7 @@
         <v>5</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -684,7 +688,29 @@
         <v>5</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added default congregate homeless tier
</commit_message>
<xml_diff>
--- a/app/shiny/templates/order_tier_defaults.xlsx
+++ b/app/shiny/templates/order_tier_defaults.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\DesktopDeployR\app\shiny\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597F9639-B8E3-4160-9A5B-E8708AE5FFAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D01CE1-D7FC-4D67-9E2C-18D20E8ADAEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="22680" windowHeight="12240" xr2:uid="{BC889A8F-D699-4C57-8F41-18B70471A466}"/>
+    <workbookView xWindow="11100" yWindow="1485" windowWidth="18570" windowHeight="14625" xr2:uid="{BC889A8F-D699-4C57-8F41-18B70471A466}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>type</t>
   </si>
@@ -135,6 +138,18 @@
   </si>
   <si>
     <t>Dialysis</t>
+  </si>
+  <si>
+    <t>Homeless Shelter</t>
+  </si>
+  <si>
+    <t>congregate, homeless</t>
+  </si>
+  <si>
+    <t>Endocrinology</t>
+  </si>
+  <si>
+    <t>Child care</t>
   </si>
 </sst>
 </file>
@@ -486,7 +501,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B3EFE4-6916-41B6-9807-EC4A4D8D59DA}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -540,7 +555,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -551,18 +566,18 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -573,7 +588,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -581,10 +599,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -592,45 +610,45 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -638,32 +656,26 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -671,10 +683,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -682,10 +694,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -693,10 +705,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -704,18 +716,56 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
         <v>5</v>
       </c>
-      <c r="C21">
+      <c r="C22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C20">
-    <sortCondition ref="A2:A20"/>
+  <autoFilter ref="A1:C1" xr:uid="{C396BBE5-9E8A-407D-A9C2-74BBCB8F360C}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C24">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C21">
+    <sortCondition ref="A2:A21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added input for 3rd order/tier sheet
</commit_message>
<xml_diff>
--- a/app/shiny/templates/order_tier_defaults.xlsx
+++ b/app/shiny/templates/order_tier_defaults.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\DesktopDeployR\app\shiny\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahu.PH\Documents\GitHub\ppe_allocatoR\app\shiny\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D01CE1-D7FC-4D67-9E2C-18D20E8ADAEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC0D838-E002-460C-B0AD-B78553BF82A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11100" yWindow="1485" windowWidth="18570" windowHeight="14625" xr2:uid="{BC889A8F-D699-4C57-8F41-18B70471A466}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BC889A8F-D699-4C57-8F41-18B70471A466}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t>type</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>Child care</t>
+  </si>
+  <si>
+    <t>School</t>
+  </si>
+  <si>
+    <t>school</t>
   </si>
 </sst>
 </file>
@@ -501,18 +507,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B3EFE4-6916-41B6-9807-EC4A4D8D59DA}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.26953125" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -523,7 +531,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -534,7 +542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -545,7 +553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -553,7 +561,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -564,7 +572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -575,7 +583,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -586,7 +594,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -597,7 +605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -608,12 +616,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -624,7 +632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -635,7 +643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -643,7 +651,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -654,7 +662,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -662,7 +670,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -670,7 +678,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -681,7 +689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -692,7 +700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -703,7 +711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -714,7 +722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -725,7 +733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -736,7 +744,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -747,7 +755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -756,6 +764,17 @@
       </c>
       <c r="C24">
         <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LTCF check error message
added error message in checking LTCFs for beds or residents
</commit_message>
<xml_diff>
--- a/app/shiny/templates/order_tier_defaults.xlsx
+++ b/app/shiny/templates/order_tier_defaults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahu.PH\Documents\GitHub\ppe_allocatoR\app\shiny\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC0D838-E002-460C-B0AD-B78553BF82A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D871D047-D421-46F9-BF5E-63B43638FCD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BC889A8F-D699-4C57-8F41-18B70471A466}"/>
+    <workbookView xWindow="1520" yWindow="0" windowWidth="16020" windowHeight="10800" xr2:uid="{BC889A8F-D699-4C57-8F41-18B70471A466}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>type</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>school</t>
+  </si>
+  <si>
+    <t>Disability Service</t>
+  </si>
+  <si>
+    <t>disability service</t>
   </si>
 </sst>
 </file>
@@ -507,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B3EFE4-6916-41B6-9807-EC4A4D8D59DA}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -774,6 +780,17 @@
         <v>39</v>
       </c>
       <c r="C25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update routes, tier defaults, and ltcf license numbers
</commit_message>
<xml_diff>
--- a/app/shiny/templates/order_tier_defaults.xlsx
+++ b/app/shiny/templates/order_tier_defaults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahu.PH\Documents\GitHub\ppe_allocatoR\app\shiny\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D871D047-D421-46F9-BF5E-63B43638FCD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF294ED-13C2-42AD-93D7-76D51DD81870}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="0" windowWidth="16020" windowHeight="10800" xr2:uid="{BC889A8F-D699-4C57-8F41-18B70471A466}"/>
+    <workbookView xWindow="-15900" yWindow="4335" windowWidth="2970" windowHeight="885" xr2:uid="{BC889A8F-D699-4C57-8F41-18B70471A466}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
   <si>
     <t>type</t>
   </si>
@@ -162,6 +162,21 @@
   </si>
   <si>
     <t>disability service</t>
+  </si>
+  <si>
+    <t>Adult Family Home</t>
+  </si>
+  <si>
+    <t>afh</t>
+  </si>
+  <si>
+    <t>Childcare</t>
+  </si>
+  <si>
+    <t>Nursing Home</t>
+  </si>
+  <si>
+    <t>LTC</t>
   </si>
 </sst>
 </file>
@@ -513,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B3EFE4-6916-41B6-9807-EC4A4D8D59DA}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -792,6 +807,50 @@
       </c>
       <c r="C26">
         <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update tiers according to new state prioritization guidance
</commit_message>
<xml_diff>
--- a/app/shiny/templates/order_tier_defaults.xlsx
+++ b/app/shiny/templates/order_tier_defaults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahu.PH\Documents\GitHub\ppe_allocatoR\app\shiny\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF294ED-13C2-42AD-93D7-76D51DD81870}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352107A4-E81B-424B-B697-9189BB6CB2BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15900" yWindow="4335" windowWidth="2970" windowHeight="885" xr2:uid="{BC889A8F-D699-4C57-8F41-18B70471A466}"/>
+    <workbookView xWindow="-25740" yWindow="7245" windowWidth="1980" windowHeight="585" xr2:uid="{BC889A8F-D699-4C57-8F41-18B70471A466}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>type</t>
   </si>
@@ -164,12 +164,6 @@
     <t>disability service</t>
   </si>
   <si>
-    <t>Adult Family Home</t>
-  </si>
-  <si>
-    <t>afh</t>
-  </si>
-  <si>
     <t>Childcare</t>
   </si>
   <si>
@@ -177,6 +171,21 @@
   </si>
   <si>
     <t>LTC</t>
+  </si>
+  <si>
+    <t>Disability Agency</t>
+  </si>
+  <si>
+    <t>Group Home</t>
+  </si>
+  <si>
+    <t>Home Care Services</t>
+  </si>
+  <si>
+    <t>Home Health Agency</t>
+  </si>
+  <si>
+    <t>Supported Living</t>
   </si>
 </sst>
 </file>
@@ -528,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B3EFE4-6916-41B6-9807-EC4A4D8D59DA}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -581,6 +590,9 @@
       <c r="B4" t="s">
         <v>31</v>
       </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -671,6 +683,9 @@
       <c r="B13" t="s">
         <v>31</v>
       </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -690,6 +705,9 @@
       <c r="B15" t="s">
         <v>29</v>
       </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -698,6 +716,9 @@
       <c r="B16" t="s">
         <v>6</v>
       </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
@@ -814,26 +835,26 @@
         <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
         <v>1</v>
@@ -844,12 +865,56 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>46</v>
       </c>
-      <c r="B30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30">
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update routing/region files and license numbers
Updating routing/region files and adding new license numbers to the ltcf comprehensive list
</commit_message>
<xml_diff>
--- a/app/shiny/templates/order_tier_defaults.xlsx
+++ b/app/shiny/templates/order_tier_defaults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahu.PH\Documents\GitHub\ppe_allocatoR\app\shiny\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352107A4-E81B-424B-B697-9189BB6CB2BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7C04EE-198E-43AB-9311-AF244FD030FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25740" yWindow="7245" windowWidth="1980" windowHeight="585" xr2:uid="{BC889A8F-D699-4C57-8F41-18B70471A466}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BC889A8F-D699-4C57-8F41-18B70471A466}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
   <si>
     <t>type</t>
   </si>
@@ -186,6 +186,21 @@
   </si>
   <si>
     <t>Supported Living</t>
+  </si>
+  <si>
+    <t>Dental</t>
+  </si>
+  <si>
+    <t>Mental Health Clinic</t>
+  </si>
+  <si>
+    <t>Shelter</t>
+  </si>
+  <si>
+    <t>Hospice</t>
+  </si>
+  <si>
+    <t>ASL</t>
   </si>
 </sst>
 </file>
@@ -537,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B3EFE4-6916-41B6-9807-EC4A4D8D59DA}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -915,6 +930,61 @@
         <v>1</v>
       </c>
       <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sorted facility name to fix default assignment
</commit_message>
<xml_diff>
--- a/app/shiny/templates/order_tier_defaults.xlsx
+++ b/app/shiny/templates/order_tier_defaults.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahu.PH\Documents\GitHub\ppe_allocatoR\app\shiny\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ppe_allocatoR\app\shiny\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7C04EE-198E-43AB-9311-AF244FD030FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759DF737-868E-4D5D-9BAF-F92DE4F30F4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BC889A8F-D699-4C57-8F41-18B70471A466}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{BC889A8F-D699-4C57-8F41-18B70471A466}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -554,18 +554,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B3EFE4-6916-41B6-9807-EC4A4D8D59DA}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.26953125" customWidth="1"/>
-    <col min="2" max="2" width="21.54296875" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -576,7 +576,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -587,7 +587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -598,31 +598,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>31</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>37</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -631,31 +631,31 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>32</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -664,333 +664,333 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B14" t="s">
         <v>3</v>
       </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="C14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B18" t="s">
         <v>31</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>36</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B19" t="s">
         <v>5</v>
       </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="C19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>27</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B21" t="s">
         <v>29</v>
       </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>17</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B23" t="s">
         <v>6</v>
       </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>34</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B25" t="s">
         <v>35</v>
       </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="C25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>24</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B27" t="s">
         <v>25</v>
       </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B28" t="s">
         <v>7</v>
       </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="C28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>28</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B29" t="s">
         <v>30</v>
       </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="C29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B34" t="s">
         <v>5</v>
       </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="C34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="B37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B39" t="s">
         <v>5</v>
       </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>47</v>
-      </c>
-      <c r="B32" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>50</v>
-      </c>
-      <c r="B35" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36" t="s">
-        <v>31</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>52</v>
-      </c>
-      <c r="B37" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" t="s">
-        <v>29</v>
-      </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>54</v>
-      </c>
-      <c r="B39" t="s">
-        <v>1</v>
-      </c>
       <c r="C39">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{C396BBE5-9E8A-407D-A9C2-74BBCB8F360C}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C24">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C39">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
added a few more defaults based on 01-14-2022 orders
</commit_message>
<xml_diff>
--- a/app/shiny/templates/order_tier_defaults.xlsx
+++ b/app/shiny/templates/order_tier_defaults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ppe_allocatoR\app\shiny\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759DF737-868E-4D5D-9BAF-F92DE4F30F4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE7329A-E50B-4F65-8973-429490C24E47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{BC889A8F-D699-4C57-8F41-18B70471A466}"/>
+    <workbookView xWindow="5265" yWindow="1170" windowWidth="21150" windowHeight="14295" xr2:uid="{BC889A8F-D699-4C57-8F41-18B70471A466}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="61">
   <si>
     <t>type</t>
   </si>
@@ -201,6 +201,24 @@
   </si>
   <si>
     <t>ASL</t>
+  </si>
+  <si>
+    <t>Accupuncture</t>
+  </si>
+  <si>
+    <t>Behavioral</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>govt, not ph</t>
+  </si>
+  <si>
+    <t>Outreach</t>
+  </si>
+  <si>
+    <t>community based organization</t>
   </si>
 </sst>
 </file>
@@ -552,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B3EFE4-6916-41B6-9807-EC4A4D8D59DA}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,18 +596,18 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -600,7 +618,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -611,10 +629,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -622,29 +640,29 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -655,29 +673,29 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -688,15 +706,21 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -704,21 +728,15 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -726,54 +744,54 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -781,32 +799,32 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -814,7 +832,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
         <v>29</v>
@@ -825,21 +843,21 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -847,10 +865,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -858,10 +876,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -869,21 +887,21 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -891,29 +909,29 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
         <v>1</v>
@@ -924,67 +942,111 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C34">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="C35">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="B37" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="B38" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>22</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B43" t="s">
         <v>5</v>
       </c>
-      <c r="C39">
+      <c r="C43">
         <v>2</v>
       </c>
     </row>
@@ -994,8 +1056,8 @@
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C21">
-    <sortCondition ref="A2:A21"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C24">
+    <sortCondition ref="A3:A24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>